<commit_message>
Committing directory before pulling
</commit_message>
<xml_diff>
--- a/Business Audit/2022 Jul - 2023 Jun/Q4 Apr - Jun/Mastercard Apr - Jun 2023.xlsx
+++ b/Business Audit/2022 Jul - 2023 Jun/Q4 Apr - Jun/Mastercard Apr - Jun 2023.xlsx
@@ -750,7 +750,7 @@
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>Mastercard Payment</t>
+          <t>PAYMENT RECEIVED, THANK YOU MasterCardPayment</t>
         </is>
       </c>
       <c r="C4" s="8" t="inlineStr"/>
@@ -798,7 +798,7 @@
       <c r="A6" s="7" t="inlineStr"/>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>Mastercard Payment</t>
+          <t>PAYMENT RECEIVED, THANK YOU MasterCardPayment</t>
         </is>
       </c>
       <c r="C6" s="8" t="inlineStr"/>
@@ -18127,15 +18127,15 @@
           <t>Chemist Warehouse</t>
         </is>
       </c>
-      <c r="C45" s="8" t="inlineStr"/>
+      <c r="C45" s="8" t="n">
+        <v>46.98</v>
+      </c>
       <c r="D45" s="8" t="inlineStr"/>
       <c r="E45" s="8" t="inlineStr"/>
       <c r="F45" s="8" t="inlineStr"/>
       <c r="G45" s="8" t="inlineStr"/>
       <c r="H45" s="8" t="inlineStr"/>
-      <c r="I45" s="8" t="n">
-        <v>46.98</v>
-      </c>
+      <c r="I45" s="8" t="inlineStr"/>
       <c r="J45" s="8" t="inlineStr"/>
       <c r="K45" s="8" t="inlineStr"/>
       <c r="L45" s="8" t="inlineStr"/>
@@ -19067,15 +19067,15 @@
           <t>Chemist Warehouse</t>
         </is>
       </c>
-      <c r="C76" s="8" t="inlineStr"/>
+      <c r="C76" s="8" t="n">
+        <v>75.47</v>
+      </c>
       <c r="D76" s="8" t="inlineStr"/>
       <c r="E76" s="8" t="inlineStr"/>
       <c r="F76" s="8" t="inlineStr"/>
       <c r="G76" s="8" t="inlineStr"/>
       <c r="H76" s="8" t="inlineStr"/>
-      <c r="I76" s="8" t="n">
-        <v>75.47</v>
-      </c>
+      <c r="I76" s="8" t="inlineStr"/>
       <c r="J76" s="8" t="inlineStr"/>
       <c r="K76" s="8" t="inlineStr"/>
       <c r="L76" s="8" t="inlineStr"/>
@@ -19831,15 +19831,15 @@
           <t>Chemist Warehouse</t>
         </is>
       </c>
-      <c r="C101" s="8" t="inlineStr"/>
+      <c r="C101" s="8" t="n">
+        <v>8.5</v>
+      </c>
       <c r="D101" s="8" t="inlineStr"/>
       <c r="E101" s="8" t="inlineStr"/>
       <c r="F101" s="8" t="inlineStr"/>
       <c r="G101" s="8" t="inlineStr"/>
       <c r="H101" s="8" t="inlineStr"/>
-      <c r="I101" s="8" t="n">
-        <v>8.5</v>
-      </c>
+      <c r="I101" s="8" t="inlineStr"/>
       <c r="J101" s="8" t="inlineStr"/>
       <c r="K101" s="8" t="inlineStr"/>
       <c r="L101" s="8" t="inlineStr"/>

</xml_diff>